<commit_message>
Actualización de formato de manuscrito
</commit_message>
<xml_diff>
--- a/guiasYformatos/cuadernoDeEstudios/formatos/AyudaCodigosGuion.xlsx
+++ b/guiasYformatos/cuadernoDeEstudios/formatos/AyudaCodigosGuion.xlsx
@@ -595,31 +595,31 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="9" dropStyle="combo" dx="33" fmlaLink="$I$22" fmlaRange="$I$8:$I$16" noThreeD="1" sel="9" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="9" dropStyle="combo" dx="33" fmlaLink="$I$22" fmlaRange="$I$8:$I$16" noThreeD="1" sel="5" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$J$22" fmlaRange="$J$6:$J$21" noThreeD="1" sel="15" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$J$22" fmlaRange="$J$6:$J$21" noThreeD="1" sel="9" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="9" dropStyle="combo" dx="33" fmlaLink="$I$22" fmlaRange="$I$8:$I$16" noThreeD="1" sel="9" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="9" dropStyle="combo" dx="33" fmlaLink="$I$22" fmlaRange="$I$8:$I$16" noThreeD="1" sel="5" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$J$22" fmlaRange="$J$6:$J$21" noThreeD="1" sel="15" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$J$22" fmlaRange="$J$6:$J$21" noThreeD="1" sel="9" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$46" fmlaRange="$K$6:$K$45" noThreeD="1" sel="18" val="13"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$46" fmlaRange="$K$6:$K$45" noThreeD="1" sel="13" val="5"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="33" fmlaLink="$H$22" fmlaRange="$H$6:$H$9" noThreeD="1" sel="3" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="33" fmlaLink="$H$22" fmlaRange="$H$6:$H$9" noThreeD="1" sel="2" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="33" fmlaLink="$H$22" fmlaRange="$H$6:$H$9" noThreeD="1" sel="3" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="33" fmlaLink="$H$22" fmlaRange="$H$6:$H$9" noThreeD="1" sel="2" val="0"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1302,7 +1302,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="D11" sqref="D11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.85" x14ac:dyDescent="0.45"/>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="D7" s="33" t="str">
         <f>CONCATENATE(H23,"_",I23,"_",J23,"_CO")</f>
-        <v>CS_11_15_CO</v>
+        <v>CN_07_09_CO</v>
       </c>
       <c r="E7" s="34"/>
       <c r="F7" s="4"/>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="D10" s="20" t="str">
         <f>CONCATENATE(D7,".docx")</f>
-        <v>CS_11_15_CO.docx</v>
+        <v>CN_07_09_CO.docx</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
@@ -1510,7 +1510,7 @@
       </c>
       <c r="D11" s="22" t="str">
         <f>CONCATENATE("GuiaDidactica_",D7,".docx")</f>
-        <v>GuiaDidactica_CS_11_15_CO.docx</v>
+        <v>GuiaDidactica_CN_07_09_CO.docx</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="23"/>
@@ -1534,7 +1534,7 @@
       </c>
       <c r="D12" s="24" t="str">
         <f>CONCATENATE("EsqueletoGuion_",D7,".docx")</f>
-        <v>EsqueletoGuion_CS_11_15_CO.docx</v>
+        <v>EsqueletoGuion_CN_07_09_CO.docx</v>
       </c>
       <c r="E12" s="24"/>
       <c r="F12" s="25"/>
@@ -1684,18 +1684,18 @@
       </c>
       <c r="D22" s="17" t="str">
         <f>CONCATENATE(H23,"_",I23,"_",J23,"_","CO_",K47)</f>
-        <v>CS_11_15_CO_REC180</v>
+        <v>CN_07_09_CO_REC130</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="18"/>
       <c r="H22" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I22" s="1">
+        <v>5</v>
+      </c>
+      <c r="J22" s="1">
         <v>9</v>
-      </c>
-      <c r="J22" s="1">
-        <v>15</v>
       </c>
       <c r="K22" s="1">
         <v>17</v>
@@ -1711,21 +1711,21 @@
       </c>
       <c r="D23" s="17" t="str">
         <f>CONCATENATE(D22,".docx")</f>
-        <v>CS_11_15_CO_REC180.docx</v>
+        <v>CN_07_09_CO_REC130.docx</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="18"/>
       <c r="H23" s="1" t="str">
         <f>IF(INDEX(H6:H9,H22)=H6,"MA",IF(INDEX(H6:H9,H22)=H7,"CN",IF(INDEX(H6:H9,H22)=H8,"CS",IF(INDEX(H6:H9,H22)=H9,"LE"))))</f>
-        <v>CS</v>
+        <v>CN</v>
       </c>
       <c r="I23" s="1" t="str">
         <f>CONCATENATE(IF((I22+2)&lt;10,"0",""),I22+2)</f>
-        <v>11</v>
+        <v>07</v>
       </c>
       <c r="J23" s="1" t="str">
         <f>CONCATENATE(IF(J22&lt;10,"0",""),J22)</f>
-        <v>15</v>
+        <v>09</v>
       </c>
       <c r="K23" s="1">
         <v>18</v>
@@ -1862,13 +1862,13 @@
     </row>
     <row r="46" spans="11:11" x14ac:dyDescent="0.45">
       <c r="K46" s="1">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="11:11" x14ac:dyDescent="0.45">
       <c r="K47" s="1" t="str">
         <f>CONCATENATE("REC",K46,0)</f>
-        <v>REC180</v>
+        <v>REC130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>